<commit_message>
Updated Lab Test Similarity Logic
To compare lab tests based on similar components:
Updated following Files:
omop_graph.py
grapk pkl file
excel file of icare4cvd vocabulary
</commit_message>
<xml_diff>
--- a/data/icare4cvd_vocabulary.xlsx
+++ b/data/icare4cvd_vocabulary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/komalgilani/Desktop/cmh/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E3ED7C5-3CD3-2D4F-85BC-113409B2BE78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA1455B-702A-0941-A695-9E76CAF1EBAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1320" yWindow="-21700" windowWidth="30240" windowHeight="17680" xr2:uid="{C761703D-2501-5143-AF98-6351D1CF682E}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17680" xr2:uid="{C761703D-2501-5143-AF98-6351D1CF682E}"/>
   </bookViews>
   <sheets>
     <sheet name="cross_walk" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1937" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1955" uniqueCount="251">
   <si>
     <t>concept_id</t>
   </si>
@@ -785,6 +785,12 @@
   </si>
   <si>
     <t>“Glucose measurement, blood”</t>
+  </si>
+  <si>
+    <t>Cholesterol in LDL [Mass/volume] in Serum or Plasma</t>
+  </si>
+  <si>
+    <t>Cholesterol in LDL [Moles/volume] in Serum or Plasma</t>
   </si>
 </sst>
 </file>
@@ -1363,10 +1369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB127A32-C101-A64A-B237-256340793849}">
-  <dimension ref="A1:N183"/>
+  <dimension ref="A1:N185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" zoomScale="69" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E183" sqref="E183"/>
+    <sheetView tabSelected="1" topLeftCell="A160" zoomScale="88" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B185" sqref="B185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8889,6 +8895,88 @@
         <v>36</v>
       </c>
       <c r="N183" s="29" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="184" spans="1:14" ht="17">
+      <c r="A184">
+        <v>3001308</v>
+      </c>
+      <c r="B184">
+        <v>3028437</v>
+      </c>
+      <c r="C184" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="D184" s="31" t="s">
+        <v>249</v>
+      </c>
+      <c r="E184" s="31" t="s">
+        <v>250</v>
+      </c>
+      <c r="F184">
+        <v>20250101</v>
+      </c>
+      <c r="G184">
+        <v>20990101</v>
+      </c>
+      <c r="I184" t="s">
+        <v>225</v>
+      </c>
+      <c r="J184" t="s">
+        <v>225</v>
+      </c>
+      <c r="K184" s="29" t="s">
+        <v>155</v>
+      </c>
+      <c r="L184" s="29" t="s">
+        <v>155</v>
+      </c>
+      <c r="M184" s="29" t="s">
+        <v>238</v>
+      </c>
+      <c r="N184" s="29" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="185" spans="1:14" ht="17">
+      <c r="A185">
+        <v>3028437</v>
+      </c>
+      <c r="B185">
+        <v>3001308</v>
+      </c>
+      <c r="C185" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="D185" s="31" t="s">
+        <v>250</v>
+      </c>
+      <c r="E185" s="31" t="s">
+        <v>249</v>
+      </c>
+      <c r="F185">
+        <v>20250101</v>
+      </c>
+      <c r="G185">
+        <v>20990101</v>
+      </c>
+      <c r="I185" t="s">
+        <v>225</v>
+      </c>
+      <c r="J185" t="s">
+        <v>225</v>
+      </c>
+      <c r="K185" s="29" t="s">
+        <v>155</v>
+      </c>
+      <c r="L185" s="29" t="s">
+        <v>155</v>
+      </c>
+      <c r="M185" s="29" t="s">
+        <v>238</v>
+      </c>
+      <c r="N185" s="29" t="s">
         <v>238</v>
       </c>
     </row>

</xml_diff>